<commit_message>
Still trying to make sure the tree gets pushed.
</commit_message>
<xml_diff>
--- a/Black_RF_Catch-only.xlsx
+++ b/Black_RF_Catch-only.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18048" windowHeight="10212" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18048" windowHeight="10212"/>
   </bookViews>
   <sheets>
     <sheet name="Black " sheetId="1" r:id="rId1"/>
@@ -994,7 +994,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2283,8 +2283,8 @@
   </sheetPr>
   <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="E7" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4047,17 +4047,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="F36:M36"/>
+    <mergeCell ref="Y8:AD8"/>
+    <mergeCell ref="F32:M32"/>
+    <mergeCell ref="F33:M33"/>
+    <mergeCell ref="F34:M34"/>
+    <mergeCell ref="F35:M35"/>
     <mergeCell ref="F30:M30"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="R8:V8"/>
-    <mergeCell ref="Y8:AD8"/>
-    <mergeCell ref="F32:M32"/>
-    <mergeCell ref="F33:M33"/>
-    <mergeCell ref="F34:M34"/>
-    <mergeCell ref="F35:M35"/>
-    <mergeCell ref="F36:M36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1"/>
@@ -4071,8 +4071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M24" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView topLeftCell="M18" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6178,7 +6178,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="A1:D24"/>
+      <selection sqref="A1:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished CA Decision Table runs.
</commit_message>
<xml_diff>
--- a/Black_RF_Catch-only.xlsx
+++ b/Black_RF_Catch-only.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18048" windowHeight="10212" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18048" windowHeight="10212" tabRatio="765" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Base_Runs" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="68">
   <si>
     <t>BLACK ROCKFISH</t>
   </si>
@@ -170,9 +170,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>Tag Q estimated</t>
-  </si>
-  <si>
     <t>Tag Q = 0.25</t>
   </si>
   <si>
@@ -195,12 +192,6 @@
   </si>
   <si>
     <t>Stock status</t>
-  </si>
-  <si>
-    <t>2014 Catch</t>
-  </si>
-  <si>
-    <t>State harvest guideline: 440.8 rec/139.2 comm.</t>
   </si>
   <si>
     <t>High catch</t>
@@ -546,6 +537,18 @@
       </rPr>
       <t xml:space="preserve"> = 0.16</t>
     </r>
+  </si>
+  <si>
+    <t>Base Catch</t>
+  </si>
+  <si>
+    <t>Low Q Catch</t>
+  </si>
+  <si>
+    <t>High Q catch</t>
+  </si>
+  <si>
+    <t>Tag Q =0.44</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1253,22 +1256,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1295,6 +1283,55 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1324,10 +1361,10 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1342,39 +1379,7 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1667,8 +1672,8 @@
   </sheetPr>
   <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1692,14 +1697,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1729,11 +1734,11 @@
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="22"/>
       <c r="E7" s="4"/>
     </row>
@@ -1750,33 +1755,33 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="51" t="s">
+      <c r="I8" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="53"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="61"/>
       <c r="O8" s="8"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
-      <c r="R8" s="54" t="s">
+      <c r="R8" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="S8" s="52"/>
-      <c r="T8" s="52"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="53"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="61"/>
       <c r="W8" s="19"/>
       <c r="X8" s="8"/>
-      <c r="Y8" s="54" t="s">
+      <c r="Y8" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="Z8" s="52"/>
-      <c r="AA8" s="52"/>
-      <c r="AB8" s="52"/>
-      <c r="AC8" s="52"/>
-      <c r="AD8" s="53"/>
+      <c r="Z8" s="60"/>
+      <c r="AA8" s="60"/>
+      <c r="AB8" s="60"/>
+      <c r="AC8" s="60"/>
+      <c r="AD8" s="61"/>
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -3453,16 +3458,16 @@
       <c r="E30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="55" t="s">
+      <c r="F30" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="63"/>
+      <c r="L30" s="63"/>
+      <c r="M30" s="63"/>
     </row>
     <row r="31" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="38">
@@ -3484,79 +3489,79 @@
       <c r="M31" s="17"/>
     </row>
     <row r="32" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F32" s="55" t="s">
+      <c r="F32" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
     </row>
     <row r="33" spans="6:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F33" s="55" t="s">
+      <c r="F33" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
     </row>
     <row r="34" spans="6:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F34" s="55" t="s">
+      <c r="F34" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="63"/>
     </row>
     <row r="35" spans="6:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F35" s="55" t="s">
+      <c r="F35" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="63"/>
+      <c r="J35" s="63"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="63"/>
+      <c r="M35" s="63"/>
     </row>
     <row r="36" spans="6:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F36" s="55" t="s">
+      <c r="F36" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="63"/>
+      <c r="K36" s="63"/>
+      <c r="L36" s="63"/>
+      <c r="M36" s="63"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="R8:V8"/>
+    <mergeCell ref="F36:M36"/>
     <mergeCell ref="Y8:AD8"/>
     <mergeCell ref="F32:M32"/>
     <mergeCell ref="F33:M33"/>
     <mergeCell ref="F34:M34"/>
     <mergeCell ref="F35:M35"/>
     <mergeCell ref="F30:M30"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="I8:M8"/>
-    <mergeCell ref="R8:V8"/>
-    <mergeCell ref="F36:M36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1"/>
@@ -3571,453 +3576,566 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:I35"/>
+      <selection activeCell="B26" sqref="B26:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="78" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="79"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="87" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="89"/>
+    </row>
+    <row r="2" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="81"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="80"/>
+      <c r="F2" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="80"/>
+      <c r="H2" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="80"/>
+    </row>
+    <row r="3" spans="1:9" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="84"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="91" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="92"/>
+      <c r="F3" s="91" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="92"/>
+      <c r="H3" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="76" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="77"/>
-    </row>
-    <row r="2" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="78" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="78" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="68"/>
-      <c r="H2" s="78" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="68"/>
-    </row>
-    <row r="3" spans="1:9" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="72"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="79" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="79" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="80"/>
-      <c r="H3" s="79" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="80"/>
+      <c r="I3" s="92"/>
     </row>
     <row r="4" spans="1:9" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="75">
+        <v>0.25</v>
+      </c>
+      <c r="E4" s="76"/>
+      <c r="F4" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="76"/>
+      <c r="H4" s="75">
+        <v>0.25</v>
+      </c>
+      <c r="I4" s="76"/>
+    </row>
+    <row r="5" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="84">
-        <v>0.25</v>
-      </c>
-      <c r="E4" s="85"/>
-      <c r="F4" s="84">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="84">
-        <v>0.25</v>
-      </c>
-      <c r="I4" s="85"/>
-    </row>
-    <row r="5" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="B5" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="C5" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="D5" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="E5" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="F5" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="77" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="48">
+        <v>2021</v>
+      </c>
+      <c r="C6" s="52">
+        <v>256.09399999999999</v>
+      </c>
+      <c r="D6" s="48"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="57"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="70"/>
+      <c r="B7" s="48">
+        <v>2022</v>
+      </c>
+      <c r="C7" s="52">
+        <v>257.34399999999999</v>
+      </c>
+      <c r="D7" s="48"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="57"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="70"/>
+      <c r="B8" s="48">
+        <v>2023</v>
+      </c>
+      <c r="C8" s="52">
+        <v>258.79199999999997</v>
+      </c>
+      <c r="D8" s="48"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="57"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="70"/>
+      <c r="B9" s="48">
+        <v>2024</v>
+      </c>
+      <c r="C9" s="52">
+        <v>260.06099999999998</v>
+      </c>
+      <c r="D9" s="48"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="57"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="70"/>
+      <c r="B10" s="48">
+        <v>2025</v>
+      </c>
+      <c r="C10" s="52">
+        <v>261.64100000000002</v>
+      </c>
+      <c r="D10" s="48"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="57"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="70"/>
+      <c r="B11" s="48">
+        <v>2026</v>
+      </c>
+      <c r="C11" s="52">
+        <v>263.15300000000002</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="57"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="70"/>
+      <c r="B12" s="48">
+        <v>2027</v>
+      </c>
+      <c r="C12" s="52">
+        <v>264.53500000000003</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="57"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="70"/>
+      <c r="B13" s="48">
+        <v>2028</v>
+      </c>
+      <c r="C13" s="52">
+        <v>265.45499999999998</v>
+      </c>
+      <c r="D13" s="48"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="57"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="70"/>
+      <c r="B14" s="48">
+        <v>2029</v>
+      </c>
+      <c r="C14" s="52">
+        <v>266.50799999999998</v>
+      </c>
+      <c r="D14" s="48"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="57"/>
+    </row>
+    <row r="15" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="71"/>
+      <c r="B15" s="49">
+        <v>2030</v>
+      </c>
+      <c r="C15" s="51">
+        <v>267.38200000000001</v>
+      </c>
+      <c r="D15" s="49"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="58"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="48">
+        <v>2021</v>
+      </c>
+      <c r="C16" s="52">
+        <v>347.62400000000002</v>
+      </c>
+      <c r="D16" s="48"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="57"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="70"/>
+      <c r="B17" s="48">
+        <v>2022</v>
+      </c>
+      <c r="C17" s="52">
+        <v>340.51799999999997</v>
+      </c>
+      <c r="D17" s="48"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="57"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="70"/>
+      <c r="B18" s="48">
+        <v>2023</v>
+      </c>
+      <c r="C18" s="52">
+        <v>334.39</v>
+      </c>
+      <c r="D18" s="48"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="57"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="70"/>
+      <c r="B19" s="48">
+        <v>2024</v>
+      </c>
+      <c r="C19" s="52">
+        <v>328.81900000000002</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="57"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="70"/>
+      <c r="B20" s="48">
+        <v>2025</v>
+      </c>
+      <c r="C20" s="52">
+        <v>324.41300000000001</v>
+      </c>
+      <c r="D20" s="48"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="57"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="70"/>
+      <c r="B21" s="48">
+        <v>2026</v>
+      </c>
+      <c r="C21" s="52">
+        <v>320.625</v>
+      </c>
+      <c r="D21" s="48"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="57"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="70"/>
+      <c r="B22" s="48">
+        <v>2027</v>
+      </c>
+      <c r="C22" s="52">
+        <v>317.31900000000002</v>
+      </c>
+      <c r="D22" s="48"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="57"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="70"/>
+      <c r="B23" s="48">
+        <v>2028</v>
+      </c>
+      <c r="C23" s="52">
+        <v>314.02999999999997</v>
+      </c>
+      <c r="D23" s="48"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="57"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="70"/>
+      <c r="B24" s="48">
+        <v>2029</v>
+      </c>
+      <c r="C24" s="52">
+        <v>311.40199999999999</v>
+      </c>
+      <c r="D24" s="48"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="57"/>
+    </row>
+    <row r="25" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="71"/>
+      <c r="B25" s="49">
+        <v>2030</v>
+      </c>
+      <c r="C25" s="51">
+        <v>309.00099999999998</v>
+      </c>
+      <c r="D25" s="49"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="58"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="60" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="90"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="86"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="90"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="86"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="90"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="86"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="90"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="86"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="90"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="90"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="86"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="90"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="86"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="90"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="86"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="90"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="86"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="90"/>
-    </row>
-    <row r="15" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="88"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="91"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="90"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="90"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="90"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="86"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="90"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="90"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="90"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="86"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="90"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="86"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="90"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="90"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="90"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="86"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="90"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="90"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="86"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="90"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="90"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="86"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="90"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="90"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="86"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="90"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="90"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="86"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="90"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="90"/>
-    </row>
-    <row r="25" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="88"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="91"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="89" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="57"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="90"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="90"/>
+      <c r="B26" s="48">
+        <v>2021</v>
+      </c>
+      <c r="C26" s="52">
+        <v>458.447</v>
+      </c>
+      <c r="D26" s="48"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="57"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="86"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="90"/>
+      <c r="A27" s="70"/>
+      <c r="B27" s="48">
+        <v>2022</v>
+      </c>
+      <c r="C27" s="52">
+        <v>438.13200000000001</v>
+      </c>
+      <c r="D27" s="48"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="57"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="86"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="90"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="90"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="90"/>
+      <c r="A28" s="70"/>
+      <c r="B28" s="48">
+        <v>2023</v>
+      </c>
+      <c r="C28" s="52">
+        <v>420.834</v>
+      </c>
+      <c r="D28" s="48"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="57"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="86"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="90"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="90"/>
+      <c r="A29" s="70"/>
+      <c r="B29" s="48">
+        <v>2024</v>
+      </c>
+      <c r="C29" s="52">
+        <v>405.86700000000002</v>
+      </c>
+      <c r="D29" s="48"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="57"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="86"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="90"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="90"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="90"/>
+      <c r="A30" s="70"/>
+      <c r="B30" s="48">
+        <v>2025</v>
+      </c>
+      <c r="C30" s="52">
+        <v>393.76600000000002</v>
+      </c>
+      <c r="D30" s="48"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="57"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="86"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="90"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="90"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="90"/>
+      <c r="A31" s="70"/>
+      <c r="B31" s="48">
+        <v>2026</v>
+      </c>
+      <c r="C31" s="52">
+        <v>383.613</v>
+      </c>
+      <c r="D31" s="48"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="57"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="86"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="90"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="90"/>
+      <c r="A32" s="70"/>
+      <c r="B32" s="48">
+        <v>2027</v>
+      </c>
+      <c r="C32" s="52">
+        <v>375.03199999999998</v>
+      </c>
+      <c r="D32" s="48"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="57"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="86"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="90"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="90"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="90"/>
+      <c r="A33" s="70"/>
+      <c r="B33" s="48">
+        <v>2028</v>
+      </c>
+      <c r="C33" s="52">
+        <v>367.291</v>
+      </c>
+      <c r="D33" s="48"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="57"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="86"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="90"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="90"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="90"/>
+      <c r="A34" s="70"/>
+      <c r="B34" s="48">
+        <v>2029</v>
+      </c>
+      <c r="C34" s="52">
+        <v>360.99400000000003</v>
+      </c>
+      <c r="D34" s="48"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="57"/>
     </row>
     <row r="35" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="88"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="91"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="91"/>
+      <c r="A35" s="71"/>
+      <c r="B35" s="49">
+        <v>2030</v>
+      </c>
+      <c r="C35" s="51">
+        <v>355.49599999999998</v>
+      </c>
+      <c r="D35" s="49"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A26:A35"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A6:A15"/>
-    <mergeCell ref="A16:A25"/>
     <mergeCell ref="A1:C3"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="D2:E2"/>
@@ -4026,6 +4144,13 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A26:A35"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A6:A15"/>
+    <mergeCell ref="A16:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4110,10 +4235,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A27:H71"/>
+  <dimension ref="A27:H77"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:D71"/>
+      <selection activeCell="A74" sqref="A74:D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4746,6 +4871,76 @@
       </c>
       <c r="D71">
         <v>235.50947641843115</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>0.12047711393793208</v>
+      </c>
+      <c r="F73">
+        <v>36.027817544795866</v>
+      </c>
+      <c r="G73">
+        <v>56.795917389907025</v>
+      </c>
+      <c r="H73">
+        <v>174.43778795135916</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2030</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>0.12047711393793208</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2030</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="D75">
+        <v>36.027817544795866</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2030</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76">
+        <v>56.795917389907025</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2030</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>4</v>
+      </c>
+      <c r="D77">
+        <v>174.43778795135916</v>
       </c>
     </row>
   </sheetData>
@@ -5249,7 +5444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A52" sqref="A52:D56"/>
     </sheetView>
   </sheetViews>
@@ -5257,19 +5452,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E1">
-        <v>6.1160573489473978E-2</v>
+        <v>1.4080685167504095E-2</v>
       </c>
       <c r="F1">
-        <v>104.34504290810619</v>
+        <v>24.022824086690651</v>
       </c>
       <c r="G1">
-        <v>131.9421965184043</v>
+        <v>30.376375228141843</v>
       </c>
       <c r="H1">
-        <v>722.87351071952969</v>
+        <v>166.42346105734066</v>
       </c>
       <c r="I1">
-        <v>25.563089280470336</v>
+        <v>5.885258942659358</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -5283,7 +5478,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>6.1160573489473978E-2</v>
+        <v>1.4080685167504095E-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5297,7 +5492,7 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <v>104.34504290810619</v>
+        <v>24.022824086690651</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -5311,7 +5506,7 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>131.9421965184043</v>
+        <v>30.376375228141843</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -5325,7 +5520,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>722.87351071952969</v>
+        <v>166.42346105734066</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -5339,24 +5534,24 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>25.563089280470336</v>
+        <v>5.885258942659358</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E7">
-        <v>5.8355143445691315E-2</v>
+        <v>1.5163681030062366E-2</v>
       </c>
       <c r="F7">
-        <v>99.558745108845486</v>
+        <v>25.870505416353019</v>
       </c>
       <c r="G7">
-        <v>125.89001974770883</v>
+        <v>32.712730902616912</v>
       </c>
       <c r="H7">
-        <v>689.71536734181518</v>
+        <v>179.22368474060875</v>
       </c>
       <c r="I7">
-        <v>24.390512658184861</v>
+        <v>6.3379152593912753</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -5370,7 +5565,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>5.8355143445691315E-2</v>
+        <v>1.5163681030062366E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -5384,7 +5579,7 @@
         <v>3</v>
       </c>
       <c r="D9">
-        <v>99.558745108845486</v>
+        <v>25.870505416353019</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -5398,7 +5593,7 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>125.89001974770883</v>
+        <v>32.712730902616912</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -5412,7 +5607,7 @@
         <v>4</v>
       </c>
       <c r="D11">
-        <v>689.71536734181518</v>
+        <v>179.22368474060875</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -5426,24 +5621,24 @@
         <v>5</v>
       </c>
       <c r="D12">
-        <v>24.390512658184861</v>
+        <v>6.3379152593912753</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13">
-        <v>5.6078852336935388E-2</v>
+        <v>1.616513235955842E-2</v>
       </c>
       <c r="F13">
-        <v>95.675202495312661</v>
+        <v>27.579064966806385</v>
       </c>
       <c r="G13">
-        <v>120.97935865235038</v>
+        <v>34.873169900834057</v>
       </c>
       <c r="H13">
-        <v>662.81126145586836</v>
+        <v>191.06011133154223</v>
       </c>
       <c r="I13">
-        <v>23.439098544131742</v>
+        <v>6.7564886684578083</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -5457,7 +5652,7 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>5.6078852336935388E-2</v>
+        <v>1.616513235955842E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -5471,7 +5666,7 @@
         <v>3</v>
       </c>
       <c r="D15">
-        <v>95.675202495312661</v>
+        <v>27.579064966806385</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -5485,7 +5680,7 @@
         <v>2</v>
       </c>
       <c r="D16">
-        <v>120.97935865235038</v>
+        <v>34.873169900834057</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -5499,7 +5694,7 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <v>662.81126145586836</v>
+        <v>191.06011133154223</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -5513,24 +5708,24 @@
         <v>5</v>
       </c>
       <c r="D18">
-        <v>23.439098544131742</v>
+        <v>6.7564886684578083</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E19">
-        <v>5.4166934248344019E-2</v>
+        <v>1.6974926088879287E-2</v>
       </c>
       <c r="F19">
-        <v>92.413310665191318</v>
+        <v>28.960640655386932</v>
       </c>
       <c r="G19">
-        <v>116.85476240056033</v>
+        <v>36.620144418524191</v>
       </c>
       <c r="H19">
-        <v>640.21377974412337</v>
+        <v>200.63128443660773</v>
       </c>
       <c r="I19">
-        <v>22.639980255876662</v>
+        <v>7.0949555633922881</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -5544,7 +5739,7 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>5.4166934248344019E-2</v>
+        <v>1.6974926088879287E-2</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -5558,7 +5753,7 @@
         <v>3</v>
       </c>
       <c r="D21">
-        <v>92.413310665191318</v>
+        <v>28.960640655386932</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -5572,7 +5767,7 @@
         <v>2</v>
       </c>
       <c r="D22">
-        <v>116.85476240056033</v>
+        <v>36.620144418524191</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -5586,7 +5781,7 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>640.21377974412337</v>
+        <v>200.63128443660773</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -5600,24 +5795,24 @@
         <v>5</v>
       </c>
       <c r="D24">
-        <v>22.639980255876662</v>
+        <v>7.0949555633922881</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E25">
-        <v>5.2632679758801662E-2</v>
+        <v>1.7582255859492735E-2</v>
       </c>
       <c r="F25">
-        <v>89.79574445530605</v>
+        <v>29.99679593252699</v>
       </c>
       <c r="G25">
-        <v>113.54490286493512</v>
+        <v>37.930341811613516</v>
       </c>
       <c r="H25">
-        <v>622.08000718583378</v>
+        <v>207.8094807549171</v>
       </c>
       <c r="I25">
-        <v>21.998712814166296</v>
+        <v>7.3487992450829305</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -5631,7 +5826,7 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <v>5.2632679758801662E-2</v>
+        <v>1.7582255859492735E-2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -5645,7 +5840,7 @@
         <v>3</v>
       </c>
       <c r="D27">
-        <v>89.79574445530605</v>
+        <v>29.99679593252699</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -5659,7 +5854,7 @@
         <v>2</v>
       </c>
       <c r="D28">
-        <v>113.54490286493512</v>
+        <v>37.930341811613516</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -5673,7 +5868,7 @@
         <v>4</v>
       </c>
       <c r="D29">
-        <v>622.08000718583378</v>
+        <v>207.8094807549171</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -5687,24 +5882,24 @@
         <v>5</v>
       </c>
       <c r="D30">
-        <v>21.998712814166296</v>
+        <v>7.3487992450829305</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E31">
-        <v>5.1461369862721318E-2</v>
+        <v>1.7883840210254461E-2</v>
       </c>
       <c r="F31">
-        <v>87.797392013659518</v>
+        <v>30.511324005519331</v>
       </c>
       <c r="G31">
-        <v>111.01802661647774</v>
+        <v>38.580952154270413</v>
       </c>
       <c r="H31">
-        <v>608.23597583668607</v>
+        <v>211.37398850844099</v>
       </c>
       <c r="I31">
-        <v>21.509144163313906</v>
+        <v>7.4748514915590283</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -5718,7 +5913,7 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>5.1461369862721318E-2</v>
+        <v>1.7883840210254461E-2</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -5732,7 +5927,7 @@
         <v>3</v>
       </c>
       <c r="D33">
-        <v>87.797392013659518</v>
+        <v>30.511324005519331</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -5746,7 +5941,7 @@
         <v>2</v>
       </c>
       <c r="D34">
-        <v>111.01802661647774</v>
+        <v>38.580952154270413</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -5760,7 +5955,7 @@
         <v>4</v>
       </c>
       <c r="D35">
-        <v>608.23597583668607</v>
+        <v>211.37398850844099</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -5774,24 +5969,24 @@
         <v>5</v>
       </c>
       <c r="D36">
-        <v>21.509144163313906</v>
+        <v>7.4748514915590283</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E37">
-        <v>5.0439734242863334E-2</v>
+        <v>1.7946007824569222E-2</v>
       </c>
       <c r="F37">
-        <v>86.054396379243542</v>
+        <v>30.617387144124216</v>
       </c>
       <c r="G37">
-        <v>108.81404388651359</v>
+        <v>38.715066848051208</v>
       </c>
       <c r="H37">
-        <v>596.16098560903617</v>
+        <v>212.10876450952776</v>
       </c>
       <c r="I37">
-        <v>21.082134390963866</v>
+        <v>7.5008354904722436</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -5805,7 +6000,7 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>5.0439734242863334E-2</v>
+        <v>1.7946007824569222E-2</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -5819,7 +6014,7 @@
         <v>3</v>
       </c>
       <c r="D39">
-        <v>86.054396379243542</v>
+        <v>30.617387144124216</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -5833,7 +6028,7 @@
         <v>2</v>
       </c>
       <c r="D40">
-        <v>108.81404388651359</v>
+        <v>38.715066848051208</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -5847,7 +6042,7 @@
         <v>4</v>
       </c>
       <c r="D41">
-        <v>596.16098560903617</v>
+        <v>212.10876450952776</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -5861,24 +6056,24 @@
         <v>5</v>
       </c>
       <c r="D42">
-        <v>21.082134390963866</v>
+        <v>7.5008354904722436</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44">
-        <v>4.9634598426702911E-2</v>
+        <v>1.7986190088766677E-2</v>
       </c>
       <c r="F44">
-        <v>84.680767479269747</v>
+        <v>30.6859414405052</v>
       </c>
       <c r="G44">
-        <v>107.07711792230354</v>
+        <v>38.801752369406032</v>
       </c>
       <c r="H44">
-        <v>586.64486565090522</v>
+        <v>212.5836896570834</v>
       </c>
       <c r="I44">
-        <v>20.745614349094808</v>
+        <v>7.5176303429166502</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -5892,7 +6087,7 @@
         <v>1</v>
       </c>
       <c r="D45">
-        <v>4.9634598426702911E-2</v>
+        <v>1.7986190088766677E-2</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -5906,7 +6101,7 @@
         <v>3</v>
       </c>
       <c r="D46">
-        <v>84.680767479269747</v>
+        <v>30.6859414405052</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -5920,7 +6115,7 @@
         <v>2</v>
       </c>
       <c r="D47">
-        <v>107.07711792230354</v>
+        <v>38.801752369406032</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -5934,7 +6129,7 @@
         <v>4</v>
       </c>
       <c r="D48">
-        <v>586.64486565090522</v>
+        <v>212.5836896570834</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -5948,24 +6143,24 @@
         <v>5</v>
       </c>
       <c r="D49">
-        <v>20.745614349094808</v>
+        <v>7.5176303429166502</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E51">
-        <v>4.8867346970914126E-2</v>
+        <v>1.7985072189608171E-2</v>
       </c>
       <c r="F51">
-        <v>83.371772459964276</v>
+        <v>30.684034211239577</v>
       </c>
       <c r="G51">
-        <v>105.42192019306481</v>
+        <v>38.799340716570811</v>
       </c>
       <c r="H51">
-        <v>577.57651128784221</v>
+        <v>212.57047690181906</v>
       </c>
       <c r="I51">
-        <v>20.424928712157886</v>
+        <v>7.5171630981809479</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -5979,7 +6174,7 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <v>4.8867346970914126E-2</v>
+        <v>1.7985072189608171E-2</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -5993,7 +6188,7 @@
         <v>3</v>
       </c>
       <c r="D53">
-        <v>83.371772459964276</v>
+        <v>30.684034211239577</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -6007,7 +6202,7 @@
         <v>2</v>
       </c>
       <c r="D54">
-        <v>105.42192019306481</v>
+        <v>38.799340716570811</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -6021,7 +6216,7 @@
         <v>4</v>
       </c>
       <c r="D55">
-        <v>577.57651128784221</v>
+        <v>212.57047690181906</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -6035,7 +6230,7 @@
         <v>5</v>
       </c>
       <c r="D56">
-        <v>20.424928712157886</v>
+        <v>7.5171630981809479</v>
       </c>
     </row>
   </sheetData>
@@ -6049,10 +6244,10 @@
     <tabColor rgb="FF00FF00"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD36"/>
+  <dimension ref="A1:AD43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6076,14 +6271,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -6113,11 +6308,11 @@
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="44"/>
       <c r="E7" s="4"/>
     </row>
@@ -6134,33 +6329,33 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="51" t="s">
+      <c r="I8" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="53"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="61"/>
       <c r="O8" s="8"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
-      <c r="R8" s="54" t="s">
+      <c r="R8" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="S8" s="52"/>
-      <c r="T8" s="52"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="53"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="61"/>
       <c r="W8" s="19"/>
       <c r="X8" s="8"/>
-      <c r="Y8" s="54" t="s">
+      <c r="Y8" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="Z8" s="52"/>
-      <c r="AA8" s="52"/>
-      <c r="AB8" s="52"/>
-      <c r="AC8" s="52"/>
-      <c r="AD8" s="53"/>
+      <c r="Z8" s="60"/>
+      <c r="AA8" s="60"/>
+      <c r="AB8" s="60"/>
+      <c r="AC8" s="60"/>
+      <c r="AD8" s="61"/>
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -6637,7 +6832,7 @@
       <c r="F15" s="10">
         <v>2020</v>
       </c>
-      <c r="G15" s="56">
+      <c r="G15" s="47">
         <f>B22</f>
         <v>0.84099999999999997</v>
       </c>
@@ -6727,7 +6922,7 @@
       <c r="F16" s="10">
         <v>2021</v>
       </c>
-      <c r="G16" s="56">
+      <c r="G16" s="47">
         <f t="shared" ref="G16:G24" si="6">B23</f>
         <v>0.83299999999999996</v>
       </c>
@@ -6827,7 +7022,7 @@
       <c r="F17" s="10">
         <v>2022</v>
       </c>
-      <c r="G17" s="56">
+      <c r="G17" s="47">
         <f t="shared" si="6"/>
         <v>0.82599999999999996</v>
       </c>
@@ -6928,7 +7123,7 @@
       <c r="F18" s="10">
         <v>2023</v>
       </c>
-      <c r="G18" s="56">
+      <c r="G18" s="47">
         <f t="shared" si="6"/>
         <v>0.81799999999999995</v>
       </c>
@@ -7028,7 +7223,7 @@
       <c r="F19" s="10">
         <v>2024</v>
       </c>
-      <c r="G19" s="56">
+      <c r="G19" s="47">
         <f t="shared" si="6"/>
         <v>0.81</v>
       </c>
@@ -7122,7 +7317,7 @@
       <c r="F20" s="10">
         <v>2025</v>
       </c>
-      <c r="G20" s="56">
+      <c r="G20" s="47">
         <f t="shared" si="6"/>
         <v>0.80300000000000005</v>
       </c>
@@ -7218,7 +7413,7 @@
       <c r="F21" s="10">
         <v>2026</v>
       </c>
-      <c r="G21" s="56">
+      <c r="G21" s="47">
         <f t="shared" si="6"/>
         <v>0.79500000000000004</v>
       </c>
@@ -7318,7 +7513,7 @@
       <c r="F22" s="10">
         <v>2027</v>
       </c>
-      <c r="G22" s="56">
+      <c r="G22" s="47">
         <f t="shared" si="6"/>
         <v>0.78800000000000003</v>
       </c>
@@ -7417,7 +7612,7 @@
       <c r="F23" s="10">
         <v>2028</v>
       </c>
-      <c r="G23" s="56">
+      <c r="G23" s="47">
         <f t="shared" si="6"/>
         <v>0.78</v>
       </c>
@@ -7516,7 +7711,7 @@
       <c r="F24" s="10">
         <v>2029</v>
       </c>
-      <c r="G24" s="56">
+      <c r="G24" s="47">
         <f t="shared" si="6"/>
         <v>0.77300000000000002</v>
       </c>
@@ -7837,16 +8032,16 @@
       <c r="E30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="55" t="s">
+      <c r="F30" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="63"/>
+      <c r="L30" s="63"/>
+      <c r="M30" s="63"/>
     </row>
     <row r="31" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="38">
@@ -7868,78 +8063,101 @@
       <c r="M31" s="45"/>
     </row>
     <row r="32" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F32" s="55" t="s">
+      <c r="F32" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-    </row>
-    <row r="33" spans="6:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F33" s="55" t="s">
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+    </row>
+    <row r="33" spans="6:18" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F33" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
-    </row>
-    <row r="34" spans="6:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F34" s="55" t="s">
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
+    </row>
+    <row r="34" spans="6:18" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F34" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-    </row>
-    <row r="35" spans="6:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F35" s="55" t="s">
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="63"/>
+    </row>
+    <row r="35" spans="6:18" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F35" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
-    </row>
-    <row r="36" spans="6:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F36" s="55" t="s">
+      <c r="G35" s="63"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="63"/>
+      <c r="J35" s="63"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="63"/>
+      <c r="M35" s="63"/>
+      <c r="R35" s="93"/>
+    </row>
+    <row r="36" spans="6:18" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F36" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="63"/>
+      <c r="K36" s="63"/>
+      <c r="L36" s="63"/>
+      <c r="M36" s="63"/>
+      <c r="R36" s="46"/>
+    </row>
+    <row r="37" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R37" s="46"/>
+    </row>
+    <row r="38" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R38" s="46"/>
+    </row>
+    <row r="39" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R39" s="93"/>
+    </row>
+    <row r="40" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R40" s="46"/>
+    </row>
+    <row r="41" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R41" s="46"/>
+    </row>
+    <row r="42" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R42" s="46"/>
+    </row>
+    <row r="43" spans="6:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R43" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="I8:M8"/>
-    <mergeCell ref="R8:V8"/>
-    <mergeCell ref="F36:M36"/>
     <mergeCell ref="Y8:AD8"/>
     <mergeCell ref="F32:M32"/>
     <mergeCell ref="F33:M33"/>
     <mergeCell ref="F34:M34"/>
     <mergeCell ref="F35:M35"/>
     <mergeCell ref="F30:M30"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="R8:V8"/>
+    <mergeCell ref="F36:M36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1"/>
@@ -7957,8 +8175,8 @@
   </sheetPr>
   <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView topLeftCell="W3" workbookViewId="0">
-      <selection activeCell="AA25" sqref="AA25"/>
+    <sheetView topLeftCell="L3" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25:V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7982,14 +8200,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -8019,11 +8237,11 @@
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="44"/>
       <c r="E7" s="4"/>
     </row>
@@ -8040,33 +8258,33 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="51" t="s">
+      <c r="I8" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="53"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="61"/>
       <c r="O8" s="8"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
-      <c r="R8" s="54" t="s">
+      <c r="R8" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="S8" s="52"/>
-      <c r="T8" s="52"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="53"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="61"/>
       <c r="W8" s="19"/>
       <c r="X8" s="8"/>
-      <c r="Y8" s="54" t="s">
+      <c r="Y8" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="Z8" s="52"/>
-      <c r="AA8" s="52"/>
-      <c r="AB8" s="52"/>
-      <c r="AC8" s="52"/>
-      <c r="AD8" s="53"/>
+      <c r="Z8" s="60"/>
+      <c r="AA8" s="60"/>
+      <c r="AB8" s="60"/>
+      <c r="AC8" s="60"/>
+      <c r="AD8" s="61"/>
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -8543,7 +8761,7 @@
       <c r="F15" s="10">
         <v>2020</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="47">
         <f>B22</f>
         <v>0.84099999999999997</v>
       </c>
@@ -8633,7 +8851,7 @@
       <c r="F16" s="10">
         <v>2021</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="47">
         <f t="shared" ref="G16:G24" si="6">B23</f>
         <v>0.83299999999999996</v>
       </c>
@@ -8731,7 +8949,7 @@
       <c r="F17" s="10">
         <v>2022</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="47">
         <f t="shared" si="6"/>
         <v>0.82599999999999996</v>
       </c>
@@ -8830,7 +9048,7 @@
       <c r="F18" s="10">
         <v>2023</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="47">
         <f t="shared" si="6"/>
         <v>0.81799999999999995</v>
       </c>
@@ -8928,7 +9146,7 @@
       <c r="F19" s="10">
         <v>2024</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="47">
         <f t="shared" si="6"/>
         <v>0.81</v>
       </c>
@@ -9020,7 +9238,7 @@
       <c r="F20" s="10">
         <v>2025</v>
       </c>
-      <c r="G20" s="31">
+      <c r="G20" s="47">
         <f t="shared" si="6"/>
         <v>0.80300000000000005</v>
       </c>
@@ -9114,7 +9332,7 @@
       <c r="F21" s="10">
         <v>2026</v>
       </c>
-      <c r="G21" s="31">
+      <c r="G21" s="47">
         <f t="shared" si="6"/>
         <v>0.79500000000000004</v>
       </c>
@@ -9212,7 +9430,7 @@
       <c r="F22" s="10">
         <v>2027</v>
       </c>
-      <c r="G22" s="31">
+      <c r="G22" s="47">
         <f t="shared" si="6"/>
         <v>0.78800000000000003</v>
       </c>
@@ -9309,7 +9527,7 @@
       <c r="F23" s="10">
         <v>2028</v>
       </c>
-      <c r="G23" s="31">
+      <c r="G23" s="47">
         <f t="shared" si="6"/>
         <v>0.78</v>
       </c>
@@ -9406,7 +9624,7 @@
       <c r="F24" s="10">
         <v>2029</v>
       </c>
-      <c r="G24" s="31">
+      <c r="G24" s="47">
         <f t="shared" si="6"/>
         <v>0.77300000000000002</v>
       </c>
@@ -9723,16 +9941,16 @@
       <c r="E30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="55" t="s">
+      <c r="F30" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="63"/>
+      <c r="L30" s="63"/>
+      <c r="M30" s="63"/>
     </row>
     <row r="31" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="38">
@@ -9754,78 +9972,78 @@
       <c r="M31" s="45"/>
     </row>
     <row r="32" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F32" s="55" t="s">
+      <c r="F32" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
     </row>
     <row r="33" spans="6:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F33" s="55" t="s">
+      <c r="F33" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
     </row>
     <row r="34" spans="6:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F34" s="55" t="s">
+      <c r="F34" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="63"/>
     </row>
     <row r="35" spans="6:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F35" s="55" t="s">
+      <c r="F35" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="63"/>
+      <c r="J35" s="63"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="63"/>
+      <c r="M35" s="63"/>
     </row>
     <row r="36" spans="6:13" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F36" s="55" t="s">
+      <c r="F36" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="63"/>
+      <c r="K36" s="63"/>
+      <c r="L36" s="63"/>
+      <c r="M36" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="I8:M8"/>
-    <mergeCell ref="R8:V8"/>
-    <mergeCell ref="F36:M36"/>
     <mergeCell ref="Y8:AD8"/>
     <mergeCell ref="F32:M32"/>
     <mergeCell ref="F33:M33"/>
     <mergeCell ref="F34:M34"/>
     <mergeCell ref="F35:M35"/>
     <mergeCell ref="F30:M30"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="R8:V8"/>
+    <mergeCell ref="F36:M36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1"/>
@@ -9839,454 +10057,567 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:I35"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="76" t="s">
+      <c r="B1" s="79"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="77"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="89"/>
     </row>
     <row r="2" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="78" t="s">
+      <c r="A2" s="81"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="78" t="s">
+      <c r="E2" s="80"/>
+      <c r="F2" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="68"/>
-      <c r="H2" s="78" t="s">
+      <c r="G2" s="80"/>
+      <c r="H2" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="68"/>
+      <c r="I2" s="80"/>
     </row>
     <row r="3" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="72"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="79" t="s">
+      <c r="A3" s="84"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="91" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="92"/>
+      <c r="F3" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="79" t="s">
+      <c r="G3" s="92"/>
+      <c r="H3" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="80"/>
-      <c r="H3" s="79" t="s">
+      <c r="I3" s="92"/>
+    </row>
+    <row r="4" spans="1:9" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="80"/>
-    </row>
-    <row r="4" spans="1:9" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="81" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="75">
+        <v>0.25</v>
+      </c>
+      <c r="E4" s="76"/>
+      <c r="F4" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="76"/>
+      <c r="H4" s="75">
+        <v>0.25</v>
+      </c>
+      <c r="I4" s="76"/>
+    </row>
+    <row r="5" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="84">
-        <v>0.25</v>
-      </c>
-      <c r="E4" s="85"/>
-      <c r="F4" s="84">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="84">
-        <v>0.25</v>
-      </c>
-      <c r="I4" s="85"/>
-    </row>
-    <row r="5" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="B5" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="C5" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="D5" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="E5" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="58" t="s">
+      <c r="H5" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="60" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="6" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="63"/>
+      <c r="A6" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="48">
+        <v>2021</v>
+      </c>
+      <c r="C6" s="52">
+        <v>226.72200000000001</v>
+      </c>
+      <c r="D6" s="53"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="54"/>
     </row>
     <row r="7" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="86"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="63"/>
+      <c r="A7" s="70"/>
+      <c r="B7" s="48">
+        <v>2022</v>
+      </c>
+      <c r="C7" s="52">
+        <v>244.16</v>
+      </c>
+      <c r="D7" s="53"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="54"/>
     </row>
     <row r="8" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="86"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="63"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="48">
+        <v>2023</v>
+      </c>
+      <c r="C8" s="52">
+        <v>260.28500000000003</v>
+      </c>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="54"/>
     </row>
     <row r="9" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="86"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="63"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="48">
+        <v>2024</v>
+      </c>
+      <c r="C9" s="52">
+        <v>273.32400000000001</v>
+      </c>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="54"/>
     </row>
     <row r="10" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="86"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="63"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="48">
+        <v>2025</v>
+      </c>
+      <c r="C10" s="52">
+        <v>283.10300000000001</v>
+      </c>
+      <c r="D10" s="53"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="54"/>
     </row>
     <row r="11" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="86"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="63"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="48">
+        <v>2026</v>
+      </c>
+      <c r="C11" s="52">
+        <v>287.959</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="54"/>
     </row>
     <row r="12" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="86"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="62"/>
-      <c r="I12" s="63"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="48">
+        <v>2027</v>
+      </c>
+      <c r="C12" s="52">
+        <v>288.95999999999998</v>
+      </c>
+      <c r="D12" s="53"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="54"/>
     </row>
     <row r="13" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="86"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="63"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="48">
+        <v>2028</v>
+      </c>
+      <c r="C13" s="52">
+        <v>289.60700000000003</v>
+      </c>
+      <c r="D13" s="53"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="54"/>
     </row>
     <row r="14" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="86"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="62"/>
-      <c r="I14" s="63"/>
+      <c r="A14" s="70"/>
+      <c r="B14" s="48">
+        <v>2029</v>
+      </c>
+      <c r="C14" s="52">
+        <v>289.589</v>
+      </c>
+      <c r="D14" s="53"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="54"/>
     </row>
     <row r="15" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="88"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="65"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="49">
+        <v>2030</v>
+      </c>
+      <c r="C15" s="51">
+        <v>289.88900000000001</v>
+      </c>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="89" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="63"/>
+      <c r="A16" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="48">
+        <v>2021</v>
+      </c>
+      <c r="C16" s="52">
+        <v>479.01100000000002</v>
+      </c>
+      <c r="D16" s="53"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="54"/>
     </row>
     <row r="17" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="86"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="63"/>
+      <c r="A17" s="70"/>
+      <c r="B17" s="48">
+        <v>2022</v>
+      </c>
+      <c r="C17" s="52">
+        <v>474.04599999999999</v>
+      </c>
+      <c r="D17" s="53"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
     </row>
     <row r="18" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="86"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="63"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="48">
+        <v>2023</v>
+      </c>
+      <c r="C18" s="52">
+        <v>470</v>
+      </c>
+      <c r="D18" s="53"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="54"/>
     </row>
     <row r="19" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="86"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="63"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="48">
+        <v>2024</v>
+      </c>
+      <c r="C19" s="52">
+        <v>465.57100000000003</v>
+      </c>
+      <c r="D19" s="53"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="54"/>
     </row>
     <row r="20" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A20" s="86"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="63"/>
+      <c r="A20" s="70"/>
+      <c r="B20" s="48">
+        <v>2025</v>
+      </c>
+      <c r="C20" s="52">
+        <v>461.29899999999998</v>
+      </c>
+      <c r="D20" s="53"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="54"/>
     </row>
     <row r="21" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A21" s="86"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="63"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="48">
+        <v>2026</v>
+      </c>
+      <c r="C21" s="52">
+        <v>457.71</v>
+      </c>
+      <c r="D21" s="53"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="54"/>
     </row>
     <row r="22" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A22" s="86"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="63"/>
+      <c r="A22" s="70"/>
+      <c r="B22" s="48">
+        <v>2027</v>
+      </c>
+      <c r="C22" s="52">
+        <v>453.61500000000001</v>
+      </c>
+      <c r="D22" s="53"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="54"/>
     </row>
     <row r="23" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A23" s="86"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="63"/>
+      <c r="A23" s="70"/>
+      <c r="B23" s="48">
+        <v>2028</v>
+      </c>
+      <c r="C23" s="52">
+        <v>450.19900000000001</v>
+      </c>
+      <c r="D23" s="53"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="54"/>
     </row>
     <row r="24" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A24" s="86"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="63"/>
+      <c r="A24" s="70"/>
+      <c r="B24" s="48">
+        <v>2029</v>
+      </c>
+      <c r="C24" s="52">
+        <v>446.28199999999998</v>
+      </c>
+      <c r="D24" s="53"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="54"/>
     </row>
     <row r="25" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="88"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="65"/>
+      <c r="A25" s="71"/>
+      <c r="B25" s="49">
+        <v>2030</v>
+      </c>
+      <c r="C25" s="51">
+        <v>443.048</v>
+      </c>
+      <c r="D25" s="55"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="56"/>
     </row>
     <row r="26" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A26" s="89" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="57"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="63"/>
+      <c r="A26" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="48">
+        <v>2021</v>
+      </c>
+      <c r="C26" s="52">
+        <v>984.78499999999997</v>
+      </c>
+      <c r="D26" s="53"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
     </row>
     <row r="27" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A27" s="86"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="63"/>
+      <c r="A27" s="70"/>
+      <c r="B27" s="48">
+        <v>2022</v>
+      </c>
+      <c r="C27" s="52">
+        <v>939.61300000000006</v>
+      </c>
+      <c r="D27" s="53"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="54"/>
     </row>
     <row r="28" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A28" s="86"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="62"/>
-      <c r="I28" s="63"/>
+      <c r="A28" s="70"/>
+      <c r="B28" s="48">
+        <v>2023</v>
+      </c>
+      <c r="C28" s="52">
+        <v>902.96100000000001</v>
+      </c>
+      <c r="D28" s="53"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="54"/>
     </row>
     <row r="29" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A29" s="86"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="63"/>
+      <c r="A29" s="70"/>
+      <c r="B29" s="48">
+        <v>2024</v>
+      </c>
+      <c r="C29" s="52">
+        <v>872.17600000000004</v>
+      </c>
+      <c r="D29" s="53"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="54"/>
     </row>
     <row r="30" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A30" s="86"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="63"/>
+      <c r="A30" s="70"/>
+      <c r="B30" s="48">
+        <v>2025</v>
+      </c>
+      <c r="C30" s="52">
+        <v>847.47199999999998</v>
+      </c>
+      <c r="D30" s="53"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="54"/>
     </row>
     <row r="31" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A31" s="86"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="63"/>
+      <c r="A31" s="70"/>
+      <c r="B31" s="48">
+        <v>2026</v>
+      </c>
+      <c r="C31" s="52">
+        <v>828.61199999999997</v>
+      </c>
+      <c r="D31" s="53"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="54"/>
     </row>
     <row r="32" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A32" s="86"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="62"/>
-      <c r="I32" s="63"/>
+      <c r="A32" s="70"/>
+      <c r="B32" s="48">
+        <v>2027</v>
+      </c>
+      <c r="C32" s="52">
+        <v>812.16200000000003</v>
+      </c>
+      <c r="D32" s="53"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="54"/>
     </row>
     <row r="33" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A33" s="86"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="63"/>
+      <c r="A33" s="70"/>
+      <c r="B33" s="48">
+        <v>2028</v>
+      </c>
+      <c r="C33" s="52">
+        <v>799.19799999999998</v>
+      </c>
+      <c r="D33" s="53"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="54"/>
     </row>
     <row r="34" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A34" s="86"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="63"/>
+      <c r="A34" s="70"/>
+      <c r="B34" s="48">
+        <v>2029</v>
+      </c>
+      <c r="C34" s="52">
+        <v>786.84400000000005</v>
+      </c>
+      <c r="D34" s="53"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="54"/>
     </row>
     <row r="35" spans="1:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="88"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="65"/>
+      <c r="A35" s="71"/>
+      <c r="B35" s="49">
+        <v>2030</v>
+      </c>
+      <c r="C35" s="51">
+        <v>776.68200000000002</v>
+      </c>
+      <c r="D35" s="55"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A26:A35"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A6:A15"/>
-    <mergeCell ref="A16:A25"/>
     <mergeCell ref="A1:C3"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="D2:E2"/>
@@ -10295,6 +10626,13 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A26:A35"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A6:A15"/>
+    <mergeCell ref="A16:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10305,453 +10643,566 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:I35"/>
+      <selection activeCell="B26" sqref="B26:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="78" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="79"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="87" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="89"/>
+    </row>
+    <row r="2" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="81"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="80"/>
+      <c r="F2" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="80"/>
+      <c r="H2" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="80"/>
+    </row>
+    <row r="3" spans="1:9" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="84"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="91" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="92"/>
+      <c r="F3" s="91" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="92"/>
+      <c r="H3" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="76" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="77"/>
-    </row>
-    <row r="2" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="78" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="78" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="68"/>
-      <c r="H2" s="78" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="68"/>
-    </row>
-    <row r="3" spans="1:9" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="72"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="79" t="s">
+      <c r="I3" s="92"/>
+    </row>
+    <row r="4" spans="1:9" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="75">
+        <v>0.25</v>
+      </c>
+      <c r="E4" s="76"/>
+      <c r="F4" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="76"/>
+      <c r="H4" s="75">
+        <v>0.25</v>
+      </c>
+      <c r="I4" s="76"/>
+    </row>
+    <row r="5" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="79" t="s">
+      <c r="B6" s="48">
+        <v>2021</v>
+      </c>
+      <c r="C6" s="52">
+        <v>188.274</v>
+      </c>
+      <c r="D6" s="48"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="57"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="70"/>
+      <c r="B7" s="48">
+        <v>2022</v>
+      </c>
+      <c r="C7" s="52">
+        <v>193.74</v>
+      </c>
+      <c r="D7" s="48"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="57"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="70"/>
+      <c r="B8" s="48">
+        <v>2023</v>
+      </c>
+      <c r="C8" s="52">
+        <v>198.82900000000001</v>
+      </c>
+      <c r="D8" s="48"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="57"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="70"/>
+      <c r="B9" s="48">
+        <v>2024</v>
+      </c>
+      <c r="C9" s="52">
+        <v>203.26900000000001</v>
+      </c>
+      <c r="D9" s="48"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="57"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="70"/>
+      <c r="B10" s="48">
+        <v>2025</v>
+      </c>
+      <c r="C10" s="52">
+        <v>207.47399999999999</v>
+      </c>
+      <c r="D10" s="48"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="57"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="70"/>
+      <c r="B11" s="48">
+        <v>2026</v>
+      </c>
+      <c r="C11" s="52">
+        <v>210.20599999999999</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="57"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="70"/>
+      <c r="B12" s="48">
+        <v>2027</v>
+      </c>
+      <c r="C12" s="52">
+        <v>212.16900000000001</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="57"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="70"/>
+      <c r="B13" s="48">
+        <v>2028</v>
+      </c>
+      <c r="C13" s="52">
+        <v>213.642</v>
+      </c>
+      <c r="D13" s="48"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="57"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="70"/>
+      <c r="B14" s="48">
+        <v>2029</v>
+      </c>
+      <c r="C14" s="52">
+        <v>215.14599999999999</v>
+      </c>
+      <c r="D14" s="48"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="57"/>
+    </row>
+    <row r="15" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="71"/>
+      <c r="B15" s="49">
+        <v>2030</v>
+      </c>
+      <c r="C15" s="51">
+        <v>216.459</v>
+      </c>
+      <c r="D15" s="49"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="58"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="80"/>
-      <c r="H3" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="80"/>
-    </row>
-    <row r="4" spans="1:9" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="81" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="84">
-        <v>0.25</v>
-      </c>
-      <c r="E4" s="85"/>
-      <c r="F4" s="84">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="84">
-        <v>0.25</v>
-      </c>
-      <c r="I4" s="85"/>
-    </row>
-    <row r="5" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="60" t="s">
+      <c r="B16" s="48">
+        <v>2021</v>
+      </c>
+      <c r="C16" s="52">
+        <v>292.56700000000001</v>
+      </c>
+      <c r="D16" s="48"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="57"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="70"/>
+      <c r="B17" s="48">
+        <v>2022</v>
+      </c>
+      <c r="C17" s="52">
+        <v>291.11500000000001</v>
+      </c>
+      <c r="D17" s="48"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="57"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="70"/>
+      <c r="B18" s="48">
+        <v>2023</v>
+      </c>
+      <c r="C18" s="52">
+        <v>289.91399999999999</v>
+      </c>
+      <c r="D18" s="48"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="57"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="70"/>
+      <c r="B19" s="48">
+        <v>2024</v>
+      </c>
+      <c r="C19" s="52">
+        <v>288.60899999999998</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="57"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="70"/>
+      <c r="B20" s="48">
+        <v>2025</v>
+      </c>
+      <c r="C20" s="52">
+        <v>287.815</v>
+      </c>
+      <c r="D20" s="48"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="57"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="70"/>
+      <c r="B21" s="48">
+        <v>2026</v>
+      </c>
+      <c r="C21" s="52">
+        <v>287.14499999999998</v>
+      </c>
+      <c r="D21" s="48"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="57"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="70"/>
+      <c r="B22" s="48">
+        <v>2027</v>
+      </c>
+      <c r="C22" s="52">
+        <v>286.54700000000003</v>
+      </c>
+      <c r="D22" s="48"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="57"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="70"/>
+      <c r="B23" s="48">
+        <v>2028</v>
+      </c>
+      <c r="C23" s="52">
+        <v>285.64999999999998</v>
+      </c>
+      <c r="D23" s="48"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="57"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="70"/>
+      <c r="B24" s="48">
+        <v>2029</v>
+      </c>
+      <c r="C24" s="52">
+        <v>285.07900000000001</v>
+      </c>
+      <c r="D24" s="48"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="57"/>
+    </row>
+    <row r="25" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="71"/>
+      <c r="B25" s="49">
+        <v>2030</v>
+      </c>
+      <c r="C25" s="51">
+        <v>284.47800000000001</v>
+      </c>
+      <c r="D25" s="49"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="58"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="60" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="87" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="90"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="86"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="90"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="86"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="90"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="86"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="90"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="86"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="90"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="90"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="86"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="90"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="86"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="90"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="86"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="90"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="86"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="90"/>
-    </row>
-    <row r="15" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="88"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="91"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="90"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="90"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="90"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="86"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="90"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="90"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="90"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="86"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="90"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="86"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="90"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="90"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="90"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="86"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="90"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="90"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="86"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="90"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="90"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="86"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="90"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="90"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="86"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="90"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="90"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="86"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="90"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="90"/>
-    </row>
-    <row r="25" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="88"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="91"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="89" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="57"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="90"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="90"/>
+      <c r="B26" s="48">
+        <v>2021</v>
+      </c>
+      <c r="C26" s="52">
+        <v>445.00700000000001</v>
+      </c>
+      <c r="D26" s="48"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="57"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="86"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="90"/>
+      <c r="A27" s="70"/>
+      <c r="B27" s="48">
+        <v>2022</v>
+      </c>
+      <c r="C27" s="52">
+        <v>434.541</v>
+      </c>
+      <c r="D27" s="48"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="57"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="86"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="90"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="90"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="90"/>
+      <c r="A28" s="70"/>
+      <c r="B28" s="48">
+        <v>2023</v>
+      </c>
+      <c r="C28" s="52">
+        <v>425.72300000000001</v>
+      </c>
+      <c r="D28" s="48"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="57"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="86"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="90"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="90"/>
+      <c r="A29" s="70"/>
+      <c r="B29" s="48">
+        <v>2024</v>
+      </c>
+      <c r="C29" s="52">
+        <v>417.92599999999999</v>
+      </c>
+      <c r="D29" s="48"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="57"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="86"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="90"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="90"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="90"/>
+      <c r="A30" s="70"/>
+      <c r="B30" s="48">
+        <v>2025</v>
+      </c>
+      <c r="C30" s="52">
+        <v>411.89800000000002</v>
+      </c>
+      <c r="D30" s="48"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="57"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="86"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="90"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="90"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="90"/>
+      <c r="A31" s="70"/>
+      <c r="B31" s="48">
+        <v>2026</v>
+      </c>
+      <c r="C31" s="52">
+        <v>406.90899999999999</v>
+      </c>
+      <c r="D31" s="48"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="57"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="86"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="90"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="90"/>
+      <c r="A32" s="70"/>
+      <c r="B32" s="48">
+        <v>2027</v>
+      </c>
+      <c r="C32" s="52">
+        <v>402.72</v>
+      </c>
+      <c r="D32" s="48"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="57"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="86"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="90"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="90"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="90"/>
+      <c r="A33" s="70"/>
+      <c r="B33" s="48">
+        <v>2028</v>
+      </c>
+      <c r="C33" s="52">
+        <v>398.65100000000001</v>
+      </c>
+      <c r="D33" s="48"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="57"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="86"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="90"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="90"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="90"/>
+      <c r="A34" s="70"/>
+      <c r="B34" s="48">
+        <v>2029</v>
+      </c>
+      <c r="C34" s="52">
+        <v>395.44799999999998</v>
+      </c>
+      <c r="D34" s="48"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="57"/>
     </row>
     <row r="35" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="88"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="91"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="91"/>
+      <c r="A35" s="71"/>
+      <c r="B35" s="49">
+        <v>2030</v>
+      </c>
+      <c r="C35" s="51">
+        <v>392.51100000000002</v>
+      </c>
+      <c r="D35" s="49"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A26:A35"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A6:A15"/>
-    <mergeCell ref="A16:A25"/>
     <mergeCell ref="A1:C3"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="D2:E2"/>
@@ -10760,6 +11211,13 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A26:A35"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A6:A15"/>
+    <mergeCell ref="A16:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>